<commit_message>
Mise à jour du README.md
</commit_message>
<xml_diff>
--- a/appweb_trpr01_grille.xlsx
+++ b/appweb_trpr01_grille.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0212c120946023de/cours/appweb_2025/02 Évaluations/trpr01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cetre\Desktop\Cegep\app_web\02_eval\TP1\tp1\appweb-trpr01-\trpr01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="666" documentId="13_ncr:1_{9ADB3289-3724-407B-9E87-4B2196B83312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9E1BAB-E015-421B-A279-8236549F36FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B22834-6E0A-4C1B-9D84-EEF1DFF3BE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grille_evaluation" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
   <si>
     <t>Éléments observables</t>
   </si>
@@ -1281,10 +1281,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_grille" displayName="tbl_grille" ref="A1:E14" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" headerRowCellStyle="Titre 1">
   <autoFilter ref="A1:E14" xr:uid="{21531910-BD78-4443-9EAB-35411D648924}"/>
@@ -1622,20 +1618,20 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="44.296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="66.296875" style="2" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.08203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.09765625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>64</v>
       </c>
@@ -1666,7 +1662,7 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26"/>
       <c r="B3" s="31" t="s">
         <v>47</v>
@@ -1678,7 +1674,7 @@
       </c>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26"/>
       <c r="B4" s="31" t="s">
         <v>48</v>
@@ -1690,7 +1686,7 @@
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26"/>
       <c r="B5" s="31" t="s">
         <v>49</v>
@@ -1702,7 +1698,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="26"/>
       <c r="B6" s="31" t="s">
         <v>50</v>
@@ -1714,7 +1710,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>61</v>
       </c>
@@ -1728,7 +1724,7 @@
       </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="47"/>
       <c r="B8" s="31" t="s">
         <v>54</v>
@@ -1740,7 +1736,7 @@
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="47"/>
       <c r="B9" s="31" t="s">
         <v>58</v>
@@ -1752,7 +1748,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26"/>
       <c r="B10" s="31" t="s">
         <v>59</v>
@@ -1764,7 +1760,7 @@
       </c>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>60</v>
       </c>
@@ -1778,7 +1774,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
       <c r="B12" s="31" t="s">
         <v>52</v>
@@ -1790,38 +1786,42 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>106</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="27" t="e">
+      <c r="C13" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="27">
         <f>VLOOKUP(C13,echelles!$A$8:$B$13,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>5</v>
       </c>
       <c r="E13" s="33"/>
     </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36"/>
       <c r="B14" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="27" t="e">
+      <c r="C14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="27">
         <f>VLOOKUP(C14,echelles!$A$8:$B$13,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>5</v>
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>14</v>
@@ -1833,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="45" t="s">
         <v>7</v>
       </c>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="E16" s="49"/>
     </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
         <v>33</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="E17" s="50"/>
     </row>
-    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
         <v>44</v>
       </c>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="E18" s="50"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
         <v>9</v>
       </c>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="E19" s="50"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="45" t="s">
         <v>17</v>
       </c>
@@ -1909,13 +1909,13 @@
       </c>
       <c r="E20" s="50"/>
     </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="42">
         <f ca="1">NOW()</f>
-        <v>45711.601906481483</v>
+        <v>45722.671391203701</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>11</v>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="E21" s="51"/>
     </row>
-    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="46" t="s">
         <v>20</v>
       </c>
@@ -1945,40 +1945,40 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
     </row>
   </sheetData>
@@ -2063,14 +2063,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.08203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="50.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>62</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2241,227 +2241,227 @@
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -2483,14 +2483,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="140.6640625" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="11.1640625" style="16"/>
+    <col min="1" max="1" width="30.19921875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="140.69921875" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="11.19921875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>23</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>22</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>32</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>28</v>
       </c>

</xml_diff>